<commit_message>
Fix equation in A1 excel
</commit_message>
<xml_diff>
--- a/NANO_KAFFEE_GmbH_YYYY_MM_Röstprotokoll_Beleg_zu_Abt1.xlsx
+++ b/NANO_KAFFEE_GmbH_YYYY_MM_Röstprotokoll_Beleg_zu_Abt1.xlsx
@@ -431,7 +431,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="14.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -689,7 +689,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="10" t="n">
-        <f aca="false">SUM(D10:D13)</f>
+        <f aca="false">D10-D11-D12-D13</f>
         <v>0</v>
       </c>
       <c r="E15" s="4"/>

</xml_diff>